<commit_message>
Edited week_1_project to V2 to be more readable and have good clear functions
</commit_message>
<xml_diff>
--- a/week_1_excel/expedia_report_monthly_march_2018.xlsx
+++ b/week_1_excel/expedia_report_monthly_march_2018.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsmouse\Desktop\AARP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\Python Lessons\SmoothStack\week_1_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA62131-740E-476D-A10B-DA1EB286520B}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C4229D-2FAE-4D05-9BF4-55087A969F88}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6210" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="2280" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary Rolling MoM" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,18 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Monthly Verbatim Statements'!$A$1:$C$413</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -3063,19 +3074,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="4" customWidth="1"/>
     <col min="4" max="4" width="9" style="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="62" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -3093,7 +3104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="104">
         <v>42842</v>
       </c>
@@ -3129,7 +3140,7 @@
       <c r="V2" s="71"/>
       <c r="W2" s="71"/>
     </row>
-    <row r="3" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="104">
         <v>42872</v>
       </c>
@@ -3159,7 +3170,7 @@
       <c r="P3" s="71"/>
       <c r="Q3" s="71"/>
     </row>
-    <row r="4" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="104">
         <v>42903</v>
       </c>
@@ -3189,7 +3200,7 @@
       <c r="P4" s="71"/>
       <c r="Q4" s="71"/>
     </row>
-    <row r="5" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="104">
         <v>42933</v>
       </c>
@@ -3219,7 +3230,7 @@
       <c r="P5" s="71"/>
       <c r="Q5" s="71"/>
     </row>
-    <row r="6" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="104">
         <v>42964</v>
       </c>
@@ -3248,7 +3259,7 @@
       <c r="P6" s="71"/>
       <c r="Q6" s="71"/>
     </row>
-    <row r="7" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="104">
         <v>42995</v>
       </c>
@@ -3277,7 +3288,7 @@
       <c r="P7" s="71"/>
       <c r="Q7" s="71"/>
     </row>
-    <row r="8" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="104">
         <v>43025</v>
       </c>
@@ -3306,7 +3317,7 @@
       <c r="P8" s="71"/>
       <c r="Q8" s="71"/>
     </row>
-    <row r="9" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="104">
         <v>43056</v>
       </c>
@@ -3341,7 +3352,7 @@
       <c r="V9" s="71"/>
       <c r="W9" s="71"/>
     </row>
-    <row r="10" spans="1:23" s="4" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="104">
         <v>43086</v>
       </c>
@@ -3377,7 +3388,7 @@
       <c r="V10" s="71"/>
       <c r="W10" s="71"/>
     </row>
-    <row r="11" spans="1:23" s="4" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="104">
         <v>43101</v>
       </c>
@@ -3399,9 +3410,9 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" spans="1:23" s="70" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" s="70" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="104">
-        <v>43149</v>
+        <v>43132</v>
       </c>
       <c r="B12" s="105">
         <v>17342</v>
@@ -3421,9 +3432,9 @@
       <c r="H12" s="71"/>
       <c r="I12" s="71"/>
     </row>
-    <row r="13" spans="1:23" s="70" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" s="70" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="104">
-        <v>43177</v>
+        <v>43160</v>
       </c>
       <c r="B13" s="105">
         <v>22343</v>
@@ -3443,7 +3454,7 @@
       <c r="H13" s="71"/>
       <c r="I13" s="71"/>
     </row>
-    <row r="14" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="107" t="s">
         <v>20</v>
       </c>
@@ -3470,11 +3481,11 @@
       <c r="I14" s="5"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="I15" s="5"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="72" t="s">
         <v>21</v>
       </c>
@@ -3487,7 +3498,7 @@
       <c r="I16" s="71"/>
       <c r="J16" s="70"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="70" t="s">
         <v>22</v>
       </c>
@@ -3500,7 +3511,7 @@
       <c r="I17" s="71"/>
       <c r="J17" s="70"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="70" t="s">
         <v>23</v>
       </c>
@@ -3513,7 +3524,7 @@
       <c r="I18" s="71"/>
       <c r="J18" s="70"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="70" t="s">
         <v>24</v>
       </c>
@@ -3526,51 +3537,51 @@
       <c r="I19" s="71"/>
       <c r="J19" s="70"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I20" s="5"/>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I21" s="5"/>
       <c r="J21" s="4"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I22" s="5"/>
       <c r="J22" s="4"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I23" s="5"/>
       <c r="J23" s="4"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I24" s="5"/>
       <c r="J24" s="4"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I25" s="5"/>
       <c r="J25" s="4"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I26" s="5"/>
       <c r="J26" s="4"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I27" s="5"/>
       <c r="J27" s="4"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I28" s="5"/>
       <c r="J28" s="4"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I29" s="5"/>
       <c r="J29" s="4"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I30" s="5"/>
       <c r="J30" s="4"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I31" s="5"/>
       <c r="J31" s="4"/>
     </row>
@@ -3585,64 +3596,61 @@
   <dimension ref="A1:BN27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.44140625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="70" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" style="70" customWidth="1"/>
-    <col min="4" max="5" width="15.26953125" style="70" customWidth="1"/>
-    <col min="6" max="16" width="15.7265625" style="70" customWidth="1"/>
-    <col min="17" max="17" width="13.1796875" style="4" customWidth="1"/>
-    <col min="18" max="23" width="13.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.1796875" style="4" customWidth="1"/>
-    <col min="27" max="27" width="38.26953125" style="29" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="12.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" style="70" customWidth="1"/>
+    <col min="4" max="5" width="15.21875" style="70" customWidth="1"/>
+    <col min="6" max="16" width="15.77734375" style="70" customWidth="1"/>
+    <col min="17" max="17" width="13.21875" style="4" customWidth="1"/>
+    <col min="18" max="23" width="13.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.21875" style="4" customWidth="1"/>
+    <col min="27" max="27" width="38.21875" style="29" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="12.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="12.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.77734375" style="4" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="13.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="12.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="12.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="12.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="10.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="45" max="46" width="12.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="12.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10.77734375" style="4" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="13.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="12.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="13.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="12.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="11.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="12.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="12.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="12.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="12.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="12.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="10.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="13.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="12.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="13.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="12.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="11.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="12.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="12.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="57" max="58" width="12.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="12.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="10.77734375" style="4" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="13.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="12.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="13.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="12.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="11.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="67" max="16384" width="9.1796875" style="4"/>
+    <col min="62" max="62" width="13.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="13.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="12.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="11.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="67" max="16384" width="9.21875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:66" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="113" t="s">
         <v>31</v>
       </c>
@@ -3835,7 +3843,7 @@
         <v>41275</v>
       </c>
     </row>
-    <row r="2" spans="1:66" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:66" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
@@ -3900,7 +3908,7 @@
       <c r="BF2" s="12"/>
       <c r="BG2" s="14"/>
     </row>
-    <row r="3" spans="1:66" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:66" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="48" t="s">
         <v>6</v>
       </c>
@@ -4098,7 +4106,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="4" spans="1:66" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:66" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="121" t="s">
         <v>7</v>
       </c>
@@ -4296,7 +4304,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:66" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:66" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="122"/>
       <c r="B5" s="95">
         <v>0.54900000000000004</v>
@@ -4492,7 +4500,7 @@
         <v>6.3E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:66" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:66" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="125" t="s">
         <v>9</v>
       </c>
@@ -4690,7 +4698,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:66" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:66" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="125"/>
       <c r="B7" s="23">
         <v>0.17100000000000001</v>
@@ -4885,7 +4893,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:66" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:66" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="125" t="s">
         <v>11</v>
       </c>
@@ -5083,7 +5091,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:66" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:66" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="125"/>
       <c r="B9" s="23">
         <v>0.26800000000000002</v>
@@ -5278,7 +5286,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:66" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:66" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="114"/>
       <c r="B10" s="115"/>
       <c r="C10" s="115"/>
@@ -5426,7 +5434,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:66" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:66" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="117"/>
       <c r="B11" s="118"/>
       <c r="C11" s="118"/>
@@ -5573,7 +5581,7 @@
         <v>0.219</v>
       </c>
     </row>
-    <row r="12" spans="1:66" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:66" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="49" t="s">
         <v>14</v>
       </c>
@@ -5723,7 +5731,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="13" spans="1:66" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:66" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="24" t="s">
         <v>16</v>
       </c>
@@ -5923,7 +5931,7 @@
         <v>0.622</v>
       </c>
     </row>
-    <row r="14" spans="1:66" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:66" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="51"/>
       <c r="B14" s="51"/>
       <c r="C14" s="51"/>
@@ -5957,7 +5965,7 @@
       <c r="Y14" s="51"/>
       <c r="Z14" s="28"/>
     </row>
-    <row r="15" spans="1:66" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:66" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="49" t="s">
         <v>17</v>
       </c>
@@ -6029,7 +6037,7 @@
       <c r="BM15" s="32"/>
       <c r="BN15" s="33"/>
     </row>
-    <row r="16" spans="1:66" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:66" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="24" t="s">
         <v>16</v>
       </c>
@@ -6227,7 +6235,7 @@
         <v>0.76500000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:66" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:66" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="52"/>
       <c r="B17" s="52"/>
       <c r="C17" s="52"/>
@@ -6295,7 +6303,7 @@
       <c r="BM17" s="38"/>
       <c r="BN17" s="38"/>
     </row>
-    <row r="18" spans="1:66" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:66" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="49" t="s">
         <v>18</v>
       </c>
@@ -6367,7 +6375,7 @@
       <c r="BM18" s="32"/>
       <c r="BN18" s="33"/>
     </row>
-    <row r="19" spans="1:66" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:66" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="24" t="s">
         <v>16</v>
       </c>
@@ -6565,7 +6573,7 @@
         <v>0.123</v>
       </c>
     </row>
-    <row r="20" spans="1:66" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:66" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="51"/>
       <c r="B20" s="51"/>
       <c r="C20" s="51"/>
@@ -6594,7 +6602,7 @@
       <c r="Z20" s="28"/>
       <c r="AA20" s="4"/>
     </row>
-    <row r="21" spans="1:66" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:66" ht="21" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="60"/>
       <c r="B21" s="60"/>
       <c r="C21" s="60"/>
@@ -6664,7 +6672,7 @@
       <c r="BM21" s="32"/>
       <c r="BN21" s="33"/>
     </row>
-    <row r="22" spans="1:66" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:66" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="59"/>
       <c r="B22" s="59"/>
       <c r="C22" s="59"/>
@@ -6812,7 +6820,7 @@
         <v>0.84799999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A23" s="61"/>
       <c r="B23" s="61"/>
       <c r="C23" s="61"/>
@@ -6840,7 +6848,7 @@
       <c r="Y23" s="68"/>
       <c r="AA23" s="45"/>
     </row>
-    <row r="24" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A24" s="53"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -6868,7 +6876,7 @@
       <c r="Y24" s="54"/>
       <c r="AA24" s="46"/>
     </row>
-    <row r="25" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A25" s="55"/>
       <c r="B25" s="56"/>
       <c r="C25" s="56"/>
@@ -6895,10 +6903,10 @@
       <c r="X25" s="56"/>
       <c r="Y25" s="58"/>
     </row>
-    <row r="26" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:66" x14ac:dyDescent="0.3">
       <c r="W26" s="5"/>
     </row>
-    <row r="27" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:66" x14ac:dyDescent="0.3">
       <c r="W27" s="5"/>
     </row>
   </sheetData>
@@ -6922,21 +6930,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E413"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" style="102" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="255.54296875" style="70" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.1796875" style="70" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.7265625" style="70" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="70"/>
+    <col min="1" max="1" width="10.77734375" style="76" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" style="102" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.5546875" style="70" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.21875" style="70" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.77734375" style="70" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.77734375" style="70"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="103" t="s">
         <v>26</v>
       </c>
@@ -6949,7 +6957,7 @@
       <c r="D1" s="79"/>
       <c r="E1" s="79"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="76">
         <v>43160.482638888898</v>
       </c>
@@ -6960,7 +6968,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="76">
         <v>43160.610416666699</v>
       </c>
@@ -6971,7 +6979,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="76">
         <v>43160.600694444402</v>
       </c>
@@ -6982,7 +6990,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="76">
         <v>43160.606249999997</v>
       </c>
@@ -6993,7 +7001,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="76">
         <v>43160.632638888899</v>
       </c>
@@ -7004,7 +7012,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="76">
         <v>43160.642361111102</v>
       </c>
@@ -7015,7 +7023,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="76">
         <v>43160.654166666704</v>
       </c>
@@ -7026,7 +7034,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="76">
         <v>43160.640277777798</v>
       </c>
@@ -7037,7 +7045,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="76">
         <v>43160.675694444399</v>
       </c>
@@ -7048,7 +7056,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="76">
         <v>43160.745833333298</v>
       </c>
@@ -7059,7 +7067,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="76">
         <v>43160.770833333299</v>
       </c>
@@ -7070,7 +7078,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="76">
         <v>43160.819444444402</v>
       </c>
@@ -7081,7 +7089,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="76">
         <v>43160.829861111102</v>
       </c>
@@ -7092,7 +7100,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="76">
         <v>43160.831250000003</v>
       </c>
@@ -7103,7 +7111,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="76">
         <v>43160.883333333302</v>
       </c>
@@ -7114,7 +7122,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="76">
         <v>43160.8659722222</v>
       </c>
@@ -7125,7 +7133,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="76">
         <v>43160.945833333302</v>
       </c>
@@ -7136,7 +7144,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="76">
         <v>43161.35</v>
       </c>
@@ -7147,7 +7155,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="76">
         <v>43161.322916666701</v>
       </c>
@@ -7158,7 +7166,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="76">
         <v>43161.499305555597</v>
       </c>
@@ -7169,7 +7177,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="76">
         <v>43161.609722222202</v>
       </c>
@@ -7180,7 +7188,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="76">
         <v>43161.592361111099</v>
       </c>
@@ -7191,7 +7199,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="76">
         <v>43161.586111111101</v>
       </c>
@@ -7202,7 +7210,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="76">
         <v>43161.570138888899</v>
       </c>
@@ -7213,7 +7221,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="76">
         <v>43161.656944444403</v>
       </c>
@@ -7224,7 +7232,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="76">
         <v>43161.675694444399</v>
       </c>
@@ -7235,7 +7243,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="76">
         <v>43161.720833333296</v>
       </c>
@@ -7246,7 +7254,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="76">
         <v>43162.383333333302</v>
       </c>
@@ -7257,7 +7265,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="76">
         <v>43163.6743055556</v>
       </c>
@@ -7268,7 +7276,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="76">
         <v>43163.681944444397</v>
       </c>
@@ -7279,7 +7287,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="76">
         <v>43163.711111111101</v>
       </c>
@@ -7290,7 +7298,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="76">
         <v>43164.634722222203</v>
       </c>
@@ -7301,7 +7309,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="76">
         <v>43164.635416666701</v>
       </c>
@@ -7312,7 +7320,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="76">
         <v>43164.609722222202</v>
       </c>
@@ -7323,7 +7331,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="76">
         <v>43164.681250000001</v>
       </c>
@@ -7334,7 +7342,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="76">
         <v>43164.691666666702</v>
       </c>
@@ -7345,7 +7353,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="76">
         <v>43164.695138888899</v>
       </c>
@@ -7356,7 +7364,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="76">
         <v>43164.746527777803</v>
       </c>
@@ -7367,7 +7375,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="76">
         <v>43164.739583333299</v>
       </c>
@@ -7378,7 +7386,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="76">
         <v>43164.724999999999</v>
       </c>
@@ -7389,7 +7397,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="76">
         <v>43164.731249999997</v>
       </c>
@@ -7400,7 +7408,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="76">
         <v>43164.786111111098</v>
       </c>
@@ -7411,7 +7419,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="76">
         <v>43164.802777777797</v>
       </c>
@@ -7422,7 +7430,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="76">
         <v>43164.822916666701</v>
       </c>
@@ -7433,7 +7441,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="76">
         <v>43164.876388888901</v>
       </c>
@@ -7444,7 +7452,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="76">
         <v>43164.894444444399</v>
       </c>
@@ -7455,7 +7463,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="76">
         <v>43164.9868055556</v>
       </c>
@@ -7466,7 +7474,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="76">
         <v>43165.019444444399</v>
       </c>
@@ -7477,7 +7485,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="76">
         <v>43164.686111111099</v>
       </c>
@@ -7488,7 +7496,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="76">
         <v>43165.185416666704</v>
       </c>
@@ -7499,7 +7507,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="76">
         <v>43165.287499999999</v>
       </c>
@@ -7510,7 +7518,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="76">
         <v>43165.420138888898</v>
       </c>
@@ -7521,7 +7529,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="76">
         <v>43164.761111111096</v>
       </c>
@@ -7532,7 +7540,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="76">
         <v>43165.5090277778</v>
       </c>
@@ -7543,7 +7551,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="76">
         <v>43165.529861111099</v>
       </c>
@@ -7554,7 +7562,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="76">
         <v>43165.6027777778</v>
       </c>
@@ -7565,7 +7573,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="76">
         <v>43165.603472222203</v>
       </c>
@@ -7576,7 +7584,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="76">
         <v>43165.5847222222</v>
       </c>
@@ -7587,7 +7595,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="76">
         <v>43165.583333333299</v>
       </c>
@@ -7598,7 +7606,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="76">
         <v>43165.594444444403</v>
       </c>
@@ -7609,7 +7617,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="76">
         <v>43165.592361111099</v>
       </c>
@@ -7620,7 +7628,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="76">
         <v>43165.625694444403</v>
       </c>
@@ -7631,7 +7639,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="76">
         <v>43165.614583333299</v>
       </c>
@@ -7642,7 +7650,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="76">
         <v>43165.613194444399</v>
       </c>
@@ -7653,7 +7661,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="76">
         <v>43165.660416666702</v>
       </c>
@@ -7664,7 +7672,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="76">
         <v>43165.649305555598</v>
       </c>
@@ -7675,7 +7683,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="76">
         <v>43165.693055555603</v>
       </c>
@@ -7686,7 +7694,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="76">
         <v>43165.710416666698</v>
       </c>
@@ -7697,7 +7705,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="76">
         <v>43165.737500000003</v>
       </c>
@@ -7708,7 +7716,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="76">
         <v>43165.766666666699</v>
       </c>
@@ -7719,7 +7727,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="76">
         <v>43165.747222222199</v>
       </c>
@@ -7730,7 +7738,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="76">
         <v>43165.8569444444</v>
       </c>
@@ -7741,7 +7749,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="76">
         <v>43165.865277777797</v>
       </c>
@@ -7752,7 +7760,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="76">
         <v>43165.941666666702</v>
       </c>
@@ -7763,7 +7771,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="76">
         <v>43166.289583333302</v>
       </c>
@@ -7774,7 +7782,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="76">
         <v>43166.395138888904</v>
       </c>
@@ -7785,7 +7793,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="76">
         <v>43166.463888888902</v>
       </c>
@@ -7796,7 +7804,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="76">
         <v>43166.440972222197</v>
       </c>
@@ -7807,7 +7815,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="76">
         <v>43166.472916666702</v>
       </c>
@@ -7818,7 +7826,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="76">
         <v>43166.545833333301</v>
       </c>
@@ -7829,7 +7837,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="76">
         <v>43166.642361111102</v>
       </c>
@@ -7840,7 +7848,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="76">
         <v>43166.610416666699</v>
       </c>
@@ -7851,7 +7859,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="76">
         <v>43166.635416666701</v>
       </c>
@@ -7862,7 +7870,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="76">
         <v>43166.664583333302</v>
       </c>
@@ -7873,7 +7881,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="76">
         <v>43166.7319444444</v>
       </c>
@@ -7884,7 +7892,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="76">
         <v>43166.751388888901</v>
       </c>
@@ -7895,7 +7903,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="76">
         <v>43166.757638888899</v>
       </c>
@@ -7906,7 +7914,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="76">
         <v>43166.921527777798</v>
       </c>
@@ -7917,7 +7925,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="76">
         <v>43166.952777777798</v>
       </c>
@@ -7928,7 +7936,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="76">
         <v>43166.931944444397</v>
       </c>
@@ -7939,7 +7947,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="76">
         <v>43167.311805555597</v>
       </c>
@@ -7950,7 +7958,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="76">
         <v>43167.601388888899</v>
       </c>
@@ -7961,7 +7969,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="76">
         <v>43167.595833333296</v>
       </c>
@@ -7972,7 +7980,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="76">
         <v>43167.617361111101</v>
       </c>
@@ -7983,7 +7991,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="76">
         <v>43167.632638888899</v>
       </c>
@@ -7994,7 +8002,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="76">
         <v>43167.649305555598</v>
       </c>
@@ -8005,7 +8013,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="76">
         <v>43167.676388888904</v>
       </c>
@@ -8016,7 +8024,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="76">
         <v>43167.681250000001</v>
       </c>
@@ -8027,7 +8035,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="76">
         <v>43167.656944444403</v>
       </c>
@@ -8038,7 +8046,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="76">
         <v>43167.664583333302</v>
       </c>
@@ -8049,7 +8057,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="76">
         <v>43167.661805555603</v>
       </c>
@@ -8060,7 +8068,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="76">
         <v>43167.685416666704</v>
       </c>
@@ -8071,7 +8079,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="76">
         <v>43167.8125</v>
       </c>
@@ -8082,7 +8090,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="76">
         <v>43167.686805555597</v>
       </c>
@@ -8093,7 +8101,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="76">
         <v>43168.066666666702</v>
       </c>
@@ -8104,7 +8112,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="76">
         <v>43168.404861111099</v>
       </c>
@@ -8115,7 +8123,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="76">
         <v>43168.6</v>
       </c>
@@ -8126,7 +8134,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="76">
         <v>43168.714583333298</v>
       </c>
@@ -8137,7 +8145,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="76">
         <v>43168.801388888904</v>
       </c>
@@ -8148,7 +8156,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="76">
         <v>43168.846527777801</v>
       </c>
@@ -8159,7 +8167,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="76">
         <v>43168.8125</v>
       </c>
@@ -8170,7 +8178,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="76">
         <v>43168.831944444399</v>
       </c>
@@ -8181,7 +8189,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="76">
         <v>43169.377083333296</v>
       </c>
@@ -8192,7 +8200,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="76">
         <v>43169.469444444403</v>
       </c>
@@ -8203,7 +8211,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="76">
         <v>43169.5756944444</v>
       </c>
@@ -8214,7 +8222,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="76">
         <v>43169.609722222202</v>
       </c>
@@ -8225,7 +8233,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="76">
         <v>43169.745833333298</v>
       </c>
@@ -8236,7 +8244,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="76">
         <v>43169.792361111096</v>
       </c>
@@ -8247,7 +8255,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="76">
         <v>43170.324999999997</v>
       </c>
@@ -8258,7 +8266,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="76">
         <v>43170.931944444397</v>
       </c>
@@ -8269,7 +8277,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="76">
         <v>43171.627083333296</v>
       </c>
@@ -8280,7 +8288,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="76">
         <v>43171.622916666704</v>
       </c>
@@ -8291,7 +8299,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="76">
         <v>43171.618750000001</v>
       </c>
@@ -8302,7 +8310,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="76">
         <v>43171.622222222199</v>
       </c>
@@ -8313,7 +8321,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="76">
         <v>43171.627083333296</v>
       </c>
@@ -8324,7 +8332,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" s="76">
         <v>43171.610416666699</v>
       </c>
@@ -8335,7 +8343,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" s="76">
         <v>43171.603472222203</v>
       </c>
@@ -8346,7 +8354,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="76">
         <v>43171.634722222203</v>
       </c>
@@ -8357,7 +8365,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="76">
         <v>43171.668055555601</v>
       </c>
@@ -8368,7 +8376,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" s="76">
         <v>43171.693055555603</v>
       </c>
@@ -8379,7 +8387,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="76">
         <v>43171.7055555556</v>
       </c>
@@ -8390,7 +8398,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" s="76">
         <v>43171.720138888901</v>
       </c>
@@ -8401,7 +8409,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="76">
         <v>43171.723611111098</v>
       </c>
@@ -8412,7 +8420,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" s="76">
         <v>43171.7722222222</v>
       </c>
@@ -8423,7 +8431,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" s="76">
         <v>43171.792361111096</v>
       </c>
@@ -8434,7 +8442,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" s="76">
         <v>43171.826388888898</v>
       </c>
@@ -8445,7 +8453,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="76">
         <v>43171.829166666699</v>
       </c>
@@ -8456,7 +8464,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" s="76">
         <v>43171.862500000003</v>
       </c>
@@ -8467,7 +8475,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="76">
         <v>43171.861111111102</v>
       </c>
@@ -8478,7 +8486,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" s="76">
         <v>43171.90625</v>
       </c>
@@ -8489,7 +8497,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" s="76">
         <v>43171.900694444397</v>
       </c>
@@ -8500,7 +8508,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" s="76">
         <v>43171.914583333302</v>
       </c>
@@ -8511,7 +8519,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" s="76">
         <v>43171.930555555598</v>
       </c>
@@ -8522,7 +8530,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" s="76">
         <v>43172</v>
       </c>
@@ -8533,7 +8541,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="76">
         <v>43172.110416666699</v>
       </c>
@@ -8544,7 +8552,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" s="76">
         <v>43172.365277777797</v>
       </c>
@@ -8555,7 +8563,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="76">
         <v>43172.386111111096</v>
       </c>
@@ -8566,7 +8574,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="76">
         <v>43172.400694444397</v>
       </c>
@@ -8577,7 +8585,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" s="76">
         <v>43172.481249999997</v>
       </c>
@@ -8588,7 +8596,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" s="76">
         <v>43172.027083333298</v>
       </c>
@@ -8599,7 +8607,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" s="76">
         <v>43172.6430555556</v>
       </c>
@@ -8610,7 +8618,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" s="76">
         <v>43172.65625</v>
       </c>
@@ -8621,7 +8629,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" s="76">
         <v>43172.661805555603</v>
       </c>
@@ -8632,7 +8640,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" s="76">
         <v>43172.659027777801</v>
       </c>
@@ -8643,7 +8651,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" s="76">
         <v>43172.640972222202</v>
       </c>
@@ -8654,7 +8662,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" s="76">
         <v>43172.658333333296</v>
       </c>
@@ -8665,7 +8673,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" s="76">
         <v>43172.681250000001</v>
       </c>
@@ -8676,7 +8684,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" s="76">
         <v>43172.718055555597</v>
       </c>
@@ -8687,7 +8695,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" s="76">
         <v>43172.770138888904</v>
       </c>
@@ -8698,7 +8706,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" s="76">
         <v>43172.759722222203</v>
       </c>
@@ -8709,7 +8717,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" s="76">
         <v>43172.791666666701</v>
       </c>
@@ -8720,7 +8728,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" s="76">
         <v>43172.899305555598</v>
       </c>
@@ -8731,7 +8739,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" s="76">
         <v>43172.940277777801</v>
       </c>
@@ -8742,7 +8750,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" s="76">
         <v>43173.054861111101</v>
       </c>
@@ -8753,7 +8761,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" s="76">
         <v>43173.210416666698</v>
       </c>
@@ -8764,7 +8772,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" s="76">
         <v>43173.498611111099</v>
       </c>
@@ -8775,7 +8783,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" s="76">
         <v>43173.525694444397</v>
       </c>
@@ -8786,7 +8794,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" s="76">
         <v>43173.587500000001</v>
       </c>
@@ -8797,7 +8805,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" s="76">
         <v>43173.665972222203</v>
       </c>
@@ -8808,7 +8816,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" s="76">
         <v>43173.6784722222</v>
       </c>
@@ -8819,7 +8827,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" s="76">
         <v>43173.668749999997</v>
       </c>
@@ -8830,7 +8838,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" s="76">
         <v>43173.668055555601</v>
       </c>
@@ -8841,7 +8849,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" s="76">
         <v>43173.672916666699</v>
       </c>
@@ -8852,7 +8860,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" s="76">
         <v>43173.6784722222</v>
       </c>
@@ -8863,7 +8871,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" s="76">
         <v>43173.719444444403</v>
       </c>
@@ -8874,7 +8882,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" s="76">
         <v>43173.748611111099</v>
       </c>
@@ -8885,7 +8893,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" s="76">
         <v>43173.756944444402</v>
       </c>
@@ -8896,7 +8904,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" s="76">
         <v>43173.7319444444</v>
       </c>
@@ -8907,7 +8915,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" s="76">
         <v>43173.745833333298</v>
       </c>
@@ -8918,7 +8926,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" s="76">
         <v>43173.756944444402</v>
       </c>
@@ -8929,7 +8937,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" s="76">
         <v>43173.829166666699</v>
       </c>
@@ -8940,7 +8948,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" s="76">
         <v>43173.8305555556</v>
       </c>
@@ -8951,7 +8959,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" s="76">
         <v>43173.867361111101</v>
       </c>
@@ -8962,7 +8970,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" s="76">
         <v>43173.855555555601</v>
       </c>
@@ -8973,7 +8981,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" s="76">
         <v>43173.868750000001</v>
       </c>
@@ -8984,7 +8992,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" s="76">
         <v>43173.910416666702</v>
       </c>
@@ -8995,7 +9003,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" s="76">
         <v>43174.000694444403</v>
       </c>
@@ -9006,7 +9014,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" s="76">
         <v>43174.1118055556</v>
       </c>
@@ -9017,7 +9025,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" s="76">
         <v>43174.3618055556</v>
       </c>
@@ -9028,7 +9036,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" s="76">
         <v>43174.445833333302</v>
       </c>
@@ -9039,7 +9047,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" s="76">
         <v>43174.494444444397</v>
       </c>
@@ -9050,7 +9058,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" s="76">
         <v>43174.5444444444</v>
       </c>
@@ -9061,7 +9069,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" s="76">
         <v>43174.620138888902</v>
       </c>
@@ -9072,7 +9080,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" s="76">
         <v>43174.6430555556</v>
       </c>
@@ -9083,7 +9091,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" s="76">
         <v>43174.698611111096</v>
       </c>
@@ -9094,7 +9102,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" s="76">
         <v>43174.694444444402</v>
       </c>
@@ -9105,7 +9113,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" s="76">
         <v>43174.723611111098</v>
       </c>
@@ -9116,7 +9124,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" s="76">
         <v>43174.715277777803</v>
       </c>
@@ -9127,7 +9135,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" s="76">
         <v>43174.712500000001</v>
       </c>
@@ -9138,7 +9146,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" s="76">
         <v>43174.765277777798</v>
       </c>
@@ -9149,7 +9157,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" s="76">
         <v>43174.796527777798</v>
       </c>
@@ -9160,7 +9168,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" s="76">
         <v>43174.856249999997</v>
       </c>
@@ -9171,7 +9179,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" s="76">
         <v>43174.859027777798</v>
       </c>
@@ -9182,7 +9190,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" s="76">
         <v>43174.847916666702</v>
       </c>
@@ -9193,7 +9201,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" s="76">
         <v>43174.8305555556</v>
       </c>
@@ -9204,7 +9212,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" s="76">
         <v>43175.267361111102</v>
       </c>
@@ -9215,7 +9223,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" s="76">
         <v>43175.441666666702</v>
       </c>
@@ -9226,7 +9234,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" s="76">
         <v>43175.551388888904</v>
       </c>
@@ -9237,7 +9245,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" s="76">
         <v>43175.661111111098</v>
       </c>
@@ -9248,7 +9256,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" s="76">
         <v>43175.672222222202</v>
       </c>
@@ -9259,7 +9267,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" s="76">
         <v>43175.668055555601</v>
       </c>
@@ -9270,7 +9278,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" s="76">
         <v>43175.644444444399</v>
       </c>
@@ -9281,7 +9289,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" s="76">
         <v>43175.6784722222</v>
       </c>
@@ -9292,7 +9300,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" s="76">
         <v>43175.722222222197</v>
       </c>
@@ -9303,7 +9311,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" s="76">
         <v>43175.690277777801</v>
       </c>
@@ -9314,7 +9322,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" s="76">
         <v>43175.706250000003</v>
       </c>
@@ -9325,7 +9333,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" s="76">
         <v>43175.709027777797</v>
       </c>
@@ -9336,7 +9344,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" s="76">
         <v>43175.725694444402</v>
       </c>
@@ -9347,7 +9355,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" s="76">
         <v>43175.752777777801</v>
       </c>
@@ -9358,7 +9366,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" s="76">
         <v>43175.736111111102</v>
       </c>
@@ -9369,7 +9377,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" s="76">
         <v>43175.747222222199</v>
       </c>
@@ -9380,7 +9388,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" s="76">
         <v>43175.842361111099</v>
       </c>
@@ -9391,7 +9399,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" s="76">
         <v>43175.8881944444</v>
       </c>
@@ -9402,7 +9410,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" s="76">
         <v>43175.927777777797</v>
       </c>
@@ -9413,7 +9421,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" s="76">
         <v>43174.324999999997</v>
       </c>
@@ -9424,7 +9432,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" s="76">
         <v>43176.505555555603</v>
       </c>
@@ -9435,7 +9443,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" s="76">
         <v>43176.5</v>
       </c>
@@ -9446,7 +9454,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" s="76">
         <v>43176.524305555598</v>
       </c>
@@ -9457,7 +9465,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" s="76">
         <v>43176.759722222203</v>
       </c>
@@ -9468,7 +9476,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" s="76">
         <v>43176.8125</v>
       </c>
@@ -9479,7 +9487,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" s="76">
         <v>43177.3</v>
       </c>
@@ -9490,7 +9498,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" s="76">
         <v>43177.4868055556</v>
       </c>
@@ -9501,7 +9509,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" s="76">
         <v>43177.631944444402</v>
       </c>
@@ -9512,7 +9520,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" s="76">
         <v>43177.779166666704</v>
       </c>
@@ -9523,7 +9531,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236" s="76">
         <v>43177.820833333302</v>
       </c>
@@ -9534,7 +9542,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" s="76">
         <v>43177.887499999997</v>
       </c>
@@ -9545,7 +9553,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" s="76">
         <v>43178.642361111102</v>
       </c>
@@ -9556,7 +9564,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" s="76">
         <v>43178.640277777798</v>
       </c>
@@ -9567,7 +9575,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240" s="76">
         <v>43178.625</v>
       </c>
@@ -9578,7 +9586,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" s="76">
         <v>43178.637499999997</v>
       </c>
@@ -9589,7 +9597,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242" s="76">
         <v>43178.658333333296</v>
       </c>
@@ -9600,7 +9608,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243" s="76">
         <v>43178.652083333298</v>
       </c>
@@ -9611,7 +9619,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A244" s="76">
         <v>43178.688194444403</v>
       </c>
@@ -9622,7 +9630,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245" s="76">
         <v>43178.6652777778</v>
       </c>
@@ -9633,7 +9641,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246" s="76">
         <v>43178.7</v>
       </c>
@@ -9644,7 +9652,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A247" s="76">
         <v>43178.724305555603</v>
       </c>
@@ -9655,7 +9663,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A248" s="76">
         <v>43178.699305555601</v>
       </c>
@@ -9666,7 +9674,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A249" s="76">
         <v>43178.756249999999</v>
       </c>
@@ -9677,7 +9685,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A250" s="76">
         <v>43178.738888888904</v>
       </c>
@@ -9688,7 +9696,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A251" s="76">
         <v>43178.8</v>
       </c>
@@ -9699,7 +9707,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A252" s="76">
         <v>43178.802777777797</v>
       </c>
@@ -9710,7 +9718,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A253" s="76">
         <v>43178.809722222199</v>
       </c>
@@ -9721,7 +9729,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254" s="76">
         <v>43178.800694444399</v>
       </c>
@@ -9732,7 +9740,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A255" s="76">
         <v>43178.823611111096</v>
       </c>
@@ -9743,7 +9751,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A256" s="76">
         <v>43179.034027777801</v>
       </c>
@@ -9754,7 +9762,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A257" s="76">
         <v>43179.308333333298</v>
       </c>
@@ -9765,7 +9773,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A258" s="76">
         <v>43179.344444444403</v>
       </c>
@@ -9776,7 +9784,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A259" s="76">
         <v>43179.390972222202</v>
       </c>
@@ -9787,7 +9795,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A260" s="76">
         <v>43179.517361111102</v>
       </c>
@@ -9798,7 +9806,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A261" s="76">
         <v>43179.526388888902</v>
       </c>
@@ -9809,7 +9817,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A262" s="76">
         <v>43179.609722222202</v>
       </c>
@@ -9820,7 +9828,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A263" s="76">
         <v>43179.653472222199</v>
       </c>
@@ -9831,7 +9839,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A264" s="76">
         <v>43179.653472222199</v>
       </c>
@@ -9842,7 +9850,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A265" s="76">
         <v>43179.680555555598</v>
       </c>
@@ -9853,7 +9861,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A266" s="76">
         <v>43179.684722222199</v>
       </c>
@@ -9864,7 +9872,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A267" s="76">
         <v>43179.658333333296</v>
       </c>
@@ -9875,7 +9883,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A268" s="76">
         <v>43179.706250000003</v>
       </c>
@@ -9886,7 +9894,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A269" s="76">
         <v>43179.698611111096</v>
       </c>
@@ -9897,7 +9905,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A270" s="76">
         <v>43179.723611111098</v>
       </c>
@@ -9908,7 +9916,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A271" s="76">
         <v>43179.740277777797</v>
       </c>
@@ -9919,7 +9927,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A272" s="76">
         <v>43179.75</v>
       </c>
@@ -9930,7 +9938,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A273" s="76">
         <v>43179.947222222203</v>
       </c>
@@ -9941,7 +9949,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A274" s="76">
         <v>43179.988194444399</v>
       </c>
@@ -9952,7 +9960,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A275" s="76">
         <v>43180.023611111101</v>
       </c>
@@ -9963,7 +9971,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A276" s="76">
         <v>43180.465277777803</v>
       </c>
@@ -9974,7 +9982,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A277" s="76">
         <v>43180.877777777801</v>
       </c>
@@ -9985,7 +9993,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A278" s="76">
         <v>43181.420833333301</v>
       </c>
@@ -9996,7 +10004,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A279" s="76">
         <v>43178.942361111098</v>
       </c>
@@ -10007,7 +10015,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A280" s="76">
         <v>43181.532638888901</v>
       </c>
@@ -10018,7 +10026,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A281" s="76">
         <v>43181.578472222202</v>
       </c>
@@ -10029,7 +10037,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A282" s="76">
         <v>43181.596527777801</v>
       </c>
@@ -10040,7 +10048,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A283" s="76">
         <v>43181.692361111098</v>
       </c>
@@ -10051,7 +10059,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A284" s="76">
         <v>43181.784722222197</v>
       </c>
@@ -10062,7 +10070,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A285" s="76">
         <v>43181.815277777801</v>
       </c>
@@ -10073,7 +10081,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A286" s="76">
         <v>43181.8125</v>
       </c>
@@ -10084,7 +10092,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A287" s="76">
         <v>43181.8569444444</v>
       </c>
@@ -10095,7 +10103,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A288" s="76">
         <v>43182.661111111098</v>
       </c>
@@ -10106,7 +10114,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A289" s="76">
         <v>43182.671527777798</v>
       </c>
@@ -10117,7 +10125,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A290" s="76">
         <v>43182.651388888902</v>
       </c>
@@ -10128,7 +10136,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A291" s="76">
         <v>43182.685416666704</v>
       </c>
@@ -10139,7 +10147,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A292" s="76">
         <v>43182.686805555597</v>
       </c>
@@ -10150,7 +10158,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A293" s="76">
         <v>43182.804861111101</v>
       </c>
@@ -10161,7 +10169,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A294" s="76">
         <v>43182.849305555603</v>
       </c>
@@ -10172,7 +10180,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A295" s="76">
         <v>43182.8215277778</v>
       </c>
@@ -10183,7 +10191,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A296" s="76">
         <v>43182.828472222202</v>
       </c>
@@ -10194,7 +10202,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A297" s="76">
         <v>43182.804166666698</v>
       </c>
@@ -10205,7 +10213,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A298" s="76">
         <v>43182.827777777798</v>
       </c>
@@ -10216,7 +10224,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A299" s="76">
         <v>43182.827777777798</v>
       </c>
@@ -10227,7 +10235,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A300" s="76">
         <v>43182.851388888899</v>
       </c>
@@ -10238,7 +10246,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A301" s="76">
         <v>43182.931250000001</v>
       </c>
@@ -10249,7 +10257,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A302" s="76">
         <v>43183.009722222203</v>
       </c>
@@ -10260,7 +10268,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A303" s="76">
         <v>43183.431944444397</v>
       </c>
@@ -10271,7 +10279,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A304" s="76">
         <v>43183.501388888901</v>
       </c>
@@ -10282,7 +10290,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A305" s="76">
         <v>43183.596527777801</v>
       </c>
@@ -10293,7 +10301,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A306" s="76">
         <v>43183.6118055556</v>
       </c>
@@ -10304,7 +10312,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A307" s="76">
         <v>43183.648611111101</v>
       </c>
@@ -10315,7 +10323,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A308" s="76">
         <v>43183.881249999999</v>
       </c>
@@ -10326,7 +10334,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A309" s="76">
         <v>43183.920833333301</v>
       </c>
@@ -10337,7 +10345,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A310" s="76">
         <v>43184.223611111098</v>
       </c>
@@ -10348,7 +10356,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A311" s="76">
         <v>43182.565972222197</v>
       </c>
@@ -10359,7 +10367,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A312" s="76">
         <v>43184.909027777801</v>
       </c>
@@ -10370,7 +10378,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A313" s="76">
         <v>43185.429166666698</v>
       </c>
@@ -10381,7 +10389,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A314" s="76">
         <v>43185.477083333302</v>
       </c>
@@ -10392,7 +10400,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A315" s="76">
         <v>43185.486111111102</v>
       </c>
@@ -10403,7 +10411,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A316" s="76">
         <v>43185.704861111102</v>
       </c>
@@ -10414,7 +10422,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A317" s="76">
         <v>43185.723611111098</v>
       </c>
@@ -10425,7 +10433,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A318" s="76">
         <v>43185.709027777797</v>
       </c>
@@ -10436,7 +10444,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A319" s="76">
         <v>43185.7277777778</v>
       </c>
@@ -10447,7 +10455,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A320" s="76">
         <v>43185.752777777801</v>
       </c>
@@ -10458,7 +10466,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A321" s="76">
         <v>43185.748611111099</v>
       </c>
@@ -10469,7 +10477,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A322" s="76">
         <v>43185.775694444397</v>
       </c>
@@ -10480,7 +10488,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A323" s="76">
         <v>43185.729861111096</v>
       </c>
@@ -10491,7 +10499,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A324" s="76">
         <v>43185.728472222203</v>
       </c>
@@ -10502,7 +10510,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A325" s="76">
         <v>43185.745138888902</v>
       </c>
@@ -10513,7 +10521,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A326" s="76">
         <v>43185.802777777797</v>
       </c>
@@ -10524,7 +10532,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A327" s="76">
         <v>43185.786805555603</v>
       </c>
@@ -10535,7 +10543,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A328" s="76">
         <v>43185.795138888898</v>
       </c>
@@ -10546,7 +10554,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A329" s="76">
         <v>43185.852083333302</v>
       </c>
@@ -10557,7 +10565,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A330" s="76">
         <v>43185.8569444444</v>
       </c>
@@ -10568,7 +10576,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A331" s="76">
         <v>43185.908333333296</v>
       </c>
@@ -10579,7 +10587,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A332" s="76">
         <v>43185.983333333301</v>
       </c>
@@ -10590,7 +10598,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A333" s="76">
         <v>43185.983333333301</v>
       </c>
@@ -10601,7 +10609,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A334" s="76">
         <v>43185.96875</v>
       </c>
@@ -10612,7 +10620,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A335" s="76">
         <v>43185.968055555597</v>
       </c>
@@ -10623,7 +10631,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A336" s="76">
         <v>43186.412499999999</v>
       </c>
@@ -10634,7 +10642,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A337" s="76">
         <v>43186.440277777801</v>
       </c>
@@ -10645,7 +10653,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A338" s="76">
         <v>43186.511805555601</v>
       </c>
@@ -10656,7 +10664,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A339" s="76">
         <v>43186.638888888898</v>
       </c>
@@ -10667,7 +10675,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A340" s="76">
         <v>43186.604166666701</v>
       </c>
@@ -10678,7 +10686,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A341" s="76">
         <v>43186.629166666702</v>
       </c>
@@ -10689,7 +10697,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A342" s="76">
         <v>43186.666666666701</v>
       </c>
@@ -10700,7 +10708,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A343" s="76">
         <v>43186.6472222222</v>
       </c>
@@ -10711,7 +10719,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A344" s="76">
         <v>43186.703472222202</v>
       </c>
@@ -10722,7 +10730,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A345" s="76">
         <v>43186.773611111101</v>
       </c>
@@ -10733,7 +10741,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A346" s="76">
         <v>43186.806250000001</v>
       </c>
@@ -10744,7 +10752,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A347" s="76">
         <v>43186.814583333296</v>
       </c>
@@ -10755,7 +10763,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A348" s="76">
         <v>43186.831944444399</v>
       </c>
@@ -10766,7 +10774,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A349" s="76">
         <v>43186.898611111101</v>
       </c>
@@ -10777,7 +10785,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A350" s="76">
         <v>43186.957638888904</v>
       </c>
@@ -10788,7 +10796,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A351" s="76">
         <v>43187.400694444397</v>
       </c>
@@ -10799,7 +10807,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A352" s="76">
         <v>43187.394444444399</v>
       </c>
@@ -10810,7 +10818,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A353" s="76">
         <v>43187.522916666698</v>
       </c>
@@ -10821,7 +10829,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A354" s="76">
         <v>43187.595138888901</v>
       </c>
@@ -10832,7 +10840,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A355" s="76">
         <v>43187.713194444397</v>
       </c>
@@ -10843,7 +10851,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A356" s="76">
         <v>43187.715277777803</v>
       </c>
@@ -10854,7 +10862,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A357" s="76">
         <v>43187.728472222203</v>
       </c>
@@ -10865,7 +10873,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A358" s="76">
         <v>43187.738194444399</v>
       </c>
@@ -10876,7 +10884,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A359" s="76">
         <v>43187.7631944444</v>
       </c>
@@ -10887,7 +10895,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A360" s="76">
         <v>43187.743055555598</v>
       </c>
@@ -10898,7 +10906,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A361" s="76">
         <v>43187.758333333302</v>
       </c>
@@ -10909,7 +10917,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A362" s="76">
         <v>43187.720833333296</v>
       </c>
@@ -10920,7 +10928,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="363" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A363" s="76">
         <v>43187.745833333298</v>
       </c>
@@ -10931,7 +10939,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="364" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A364" s="76">
         <v>43187.781944444403</v>
       </c>
@@ -10942,7 +10950,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="365" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A365" s="76">
         <v>43187.790972222203</v>
       </c>
@@ -10953,7 +10961,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A366" s="76">
         <v>43187.806944444397</v>
       </c>
@@ -10964,7 +10972,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="367" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A367" s="76">
         <v>43187.780555555597</v>
       </c>
@@ -10975,7 +10983,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="368" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A368" s="76">
         <v>43187.775000000001</v>
       </c>
@@ -10986,7 +10994,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A369" s="76">
         <v>43187.847222222197</v>
       </c>
@@ -10997,7 +11005,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A370" s="76">
         <v>43187.8840277778</v>
       </c>
@@ -11008,7 +11016,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A371" s="76">
         <v>43187.870833333298</v>
       </c>
@@ -11019,7 +11027,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A372" s="76">
         <v>43187.905555555597</v>
       </c>
@@ -11030,7 +11038,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A373" s="76">
         <v>43188.002083333296</v>
       </c>
@@ -11041,7 +11049,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A374" s="76">
         <v>43186.945833333302</v>
       </c>
@@ -11052,7 +11060,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A375" s="76">
         <v>43188.086805555598</v>
       </c>
@@ -11063,7 +11071,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="376" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A376" s="76">
         <v>43188.391666666699</v>
       </c>
@@ -11074,7 +11082,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A377" s="76">
         <v>43188.368055555598</v>
       </c>
@@ -11085,7 +11093,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A378" s="76">
         <v>43188.398611111101</v>
       </c>
@@ -11096,7 +11104,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A379" s="76">
         <v>43188.434027777803</v>
       </c>
@@ -11107,7 +11115,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A380" s="76">
         <v>43188.4375</v>
       </c>
@@ -11118,7 +11126,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A381" s="76">
         <v>43188.499305555597</v>
       </c>
@@ -11129,7 +11137,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="382" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A382" s="76">
         <v>43188.636111111096</v>
       </c>
@@ -11140,7 +11148,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A383" s="76">
         <v>43188.661805555603</v>
       </c>
@@ -11151,7 +11159,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A384" s="76">
         <v>43188.722222222197</v>
       </c>
@@ -11162,7 +11170,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="385" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A385" s="76">
         <v>43188.811805555597</v>
       </c>
@@ -11173,7 +11181,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="386" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A386" s="76">
         <v>43188.876388888901</v>
       </c>
@@ -11184,7 +11192,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="387" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A387" s="76">
         <v>43188.909722222197</v>
       </c>
@@ -11195,7 +11203,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="388" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A388" s="76">
         <v>43189.015972222202</v>
       </c>
@@ -11206,7 +11214,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="389" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A389" s="76">
         <v>43189.029861111099</v>
       </c>
@@ -11217,7 +11225,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="390" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A390" s="76">
         <v>43188.477083333302</v>
       </c>
@@ -11228,7 +11236,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="391" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A391" s="76">
         <v>43189.482638888898</v>
       </c>
@@ -11239,7 +11247,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="392" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A392" s="76">
         <v>43189.586805555598</v>
       </c>
@@ -11250,7 +11258,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="393" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A393" s="76">
         <v>43189.579166666699</v>
       </c>
@@ -11261,7 +11269,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="394" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A394" s="76">
         <v>43189.616666666698</v>
       </c>
@@ -11272,7 +11280,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="395" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A395" s="76">
         <v>43189.629861111098</v>
       </c>
@@ -11283,7 +11291,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="396" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A396" s="76">
         <v>43189.599305555603</v>
       </c>
@@ -11294,7 +11302,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="397" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A397" s="76">
         <v>43189.589583333298</v>
       </c>
@@ -11305,7 +11313,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="398" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A398" s="76">
         <v>43189.6652777778</v>
       </c>
@@ -11316,7 +11324,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="399" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A399" s="76">
         <v>43189.638888888898</v>
       </c>
@@ -11327,7 +11335,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="400" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A400" s="76">
         <v>43189.667361111096</v>
       </c>
@@ -11338,7 +11346,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="401" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A401" s="76">
         <v>43189.679166666698</v>
       </c>
@@ -11349,7 +11357,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="402" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A402" s="76">
         <v>43189.706250000003</v>
       </c>
@@ -11360,7 +11368,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="403" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A403" s="76">
         <v>43189.756944444402</v>
       </c>
@@ -11371,7 +11379,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="404" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A404" s="76">
         <v>43189.782638888901</v>
       </c>
@@ -11382,7 +11390,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="405" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A405" s="76">
         <v>43189.787499999999</v>
       </c>
@@ -11393,7 +11401,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="406" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A406" s="76">
         <v>43189.785416666702</v>
       </c>
@@ -11404,7 +11412,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="407" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A407" s="76">
         <v>43189.911805555603</v>
       </c>
@@ -11415,7 +11423,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="408" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A408" s="76">
         <v>43189.882638888899</v>
       </c>
@@ -11426,7 +11434,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="409" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="409" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A409" s="76">
         <v>43189.945833333302</v>
       </c>
@@ -11437,7 +11445,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="410" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="410" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A410" s="76">
         <v>43190.246527777803</v>
       </c>
@@ -11448,7 +11456,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="411" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="411" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A411" s="76">
         <v>43190.504861111098</v>
       </c>
@@ -11459,7 +11467,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="412" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="412" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A412" s="76">
         <v>43190.556944444397</v>
       </c>
@@ -11470,7 +11478,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="413" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="413" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A413" s="76">
         <v>43190.945138888899</v>
       </c>
@@ -11672,13 +11680,37 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49C74C9C-BC27-42EB-9775-4C47E637794F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49C74C9C-BC27-42EB-9775-4C47E637794F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34A8C65B-1DBE-4DE4-B55E-F66C145F10BA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34A8C65B-1DBE-4DE4-B55E-F66C145F10BA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2987eda7-d74f-4356-b66a-f07c93829225"/>
+    <ds:schemaRef ds:uri="f34a3a25-800e-4071-8a5e-9727d3108910"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B68ADE93-5685-4700-8E6C-6ABF673C8EF3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B68ADE93-5685-4700-8E6C-6ABF673C8EF3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>